<commit_message>
Update excel for early duration
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/Config.xlsx
+++ b/attendance/src/main/resources/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t xml:space="preserve">RunMode</t>
   </si>
@@ -43,13 +43,13 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">scope:Absent</t>
+    <t xml:space="preserve">mod:LeaveDeduction</t>
   </si>
   <si>
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
-    <t xml:space="preserve">automation3</t>
+    <t xml:space="preserve">bob</t>
   </si>
   <si>
     <t xml:space="preserve">DEBUG</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">scope:EarlyDuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bob</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
@@ -206,7 +203,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,7 +268,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -285,19 +282,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,19 +302,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest changes for enhanced performance in terms of policy changes
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/Config.xlsx
+++ b/attendance/src/main/resources/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">RunMode</t>
   </si>
@@ -43,25 +43,28 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">mod:LeaveDeduction</t>
+    <t xml:space="preserve">scope:Absent</t>
   </si>
   <si>
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
+    <t xml:space="preserve">automation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeaveDeductions.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope:EarlyDuration</t>
+  </si>
+  <si>
     <t xml:space="preserve">bob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEBUG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeaveDeductions.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope:EarlyDuration</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
@@ -203,7 +206,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,7 +271,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -282,19 +285,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,19 +305,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sheet for execution
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/Config.xlsx
+++ b/attendance/src/main/resources/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t xml:space="preserve">RunMode</t>
   </si>
@@ -43,13 +43,13 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">scope:Absent</t>
+    <t xml:space="preserve">all</t>
   </si>
   <si>
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
-    <t xml:space="preserve">automation</t>
+    <t xml:space="preserve">bob</t>
   </si>
   <si>
     <t xml:space="preserve">DEBUG</t>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">scope:EarlyDuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
   </si>
   <si>
     <t xml:space="preserve">vijay</t>
@@ -206,7 +200,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,7 +265,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -285,19 +279,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,19 +299,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update settings and sort order
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/Config.xlsx
+++ b/attendance/src/main/resources/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t xml:space="preserve">RunMode</t>
   </si>
@@ -49,19 +49,22 @@
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
+    <t xml:space="preserve">automation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeaveDeductions.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope:EarlyDuration</t>
+  </si>
+  <si>
     <t xml:space="preserve">bob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEBUG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeaveDeductions.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope:EarlyDuration</t>
   </si>
   <si>
     <t xml:space="preserve">vijay</t>
@@ -200,7 +203,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:F2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -265,7 +268,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -285,13 +288,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,19 +302,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>